<commit_message>
had counter set in init when it was unnecessary. commented out test runs.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47e1dd5e922b67ff/ath/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{78240DC8-BF0F-4AAD-86EA-A46B6BB4F4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{8757CFBD-AF21-425C-AAE7-516CAD80F822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>1^4^6</t>
   </si>
@@ -346,15 +346,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -367,8 +367,11 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -381,8 +384,11 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -393,6 +399,9 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved test of my new class to tester.py and tested in test.xlsx (filled sixth column.)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47e1dd5e922b67ff/ath/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{8757CFBD-AF21-425C-AAE7-516CAD80F822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{59BAF3A8-F1A0-4465-990F-673FFE7F627F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>1^4^6</t>
   </si>
@@ -346,7 +346,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E4"/>
+  <dimension ref="A2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -354,7 +354,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -370,8 +370,11 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -387,8 +390,11 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -402,6 +408,9 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added comments to athimporter. tester exists as a blueprint to others who might want to utilize this program.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47e1dd5e922b67ff/ath/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{59BAF3A8-F1A0-4465-990F-673FFE7F627F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{5D031248-058B-42CD-AFE8-7BAA82970BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>1^4^6</t>
   </si>
@@ -346,7 +346,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A2:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -354,7 +354,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -373,8 +373,11 @@
       <c r="F2" t="s">
         <v>0</v>
       </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -393,8 +396,11 @@
       <c r="F3" t="s">
         <v>1</v>
       </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -411,6 +417,9 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>